<commit_message>
[2017.04.22] userImage zip파일 업로드로 변경
</commit_message>
<xml_diff>
--- a/association/src/main/webapp/resources/upload/excel/test4.xlsx
+++ b/association/src/main/webapp/resources/upload/excel/test4.xlsx
@@ -24,16 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>기수</t>
   </si>
   <si>
     <t>이름</t>
-  </si>
-  <si>
-    <t>사진</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>전화번호</t>
@@ -162,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +171,6 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -216,18 +205,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -246,363 +232,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1019317</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1314633</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="1584960"/>
-          <a:ext cx="1019317" cy="1276533"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1019317</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1305107</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="2926080"/>
-          <a:ext cx="1019317" cy="1274627"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1047896</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1333686</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="4244340"/>
-          <a:ext cx="1047896" cy="1310826"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1009791</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1305107</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="그림 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="5654040"/>
-          <a:ext cx="1009791" cy="1236527"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1009791</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1286054</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="그림 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="6979920"/>
-          <a:ext cx="1009791" cy="1225094"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1009791</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1314633</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="그림 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="8282940"/>
-          <a:ext cx="1009791" cy="1261293"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>99059</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1038370</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1257300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="9685019"/>
-          <a:ext cx="1038370" cy="1158241"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1038370</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1314633</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="그림 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2011680" y="274320"/>
-          <a:ext cx="1038370" cy="1261293"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -868,18 +497,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I9"/>
+  <dimension ref="B1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="4" width="14.69921875" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -901,18 +534,17 @@
       <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" ht="109.8" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>9</v>
       </c>
@@ -925,23 +557,22 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="114" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1"/>
       <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -949,161 +580,152 @@
       <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" ht="111.6" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="114" customHeight="1" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1"/>
       <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="110.4" customHeight="1" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1"/>
       <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
       </c>
       <c r="G6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="106.8" customHeight="1" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="111" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
       <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="106.8" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
       <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1"/>
-    <hyperlink ref="I8" r:id="rId2"/>
-    <hyperlink ref="I9" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId1"/>
+    <hyperlink ref="H8" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>